<commit_message>
removed sheets that were not dataset
</commit_message>
<xml_diff>
--- a/Resources/state_local_finances.xlsx
+++ b/Resources/state_local_finances.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\PFAB-A\website\2019 Release\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaming PC\Desktop\Police-Crime-Rates-vs-City-Budgets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F33049A3-ED4A-4F77-9C6A-CAE2CFC2CCEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9133763-2105-43C6-AD97-A7D8BC162730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019_US_MS" sheetId="1" r:id="rId1"/>
@@ -1361,6 +1361,15 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="4" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1387,15 +1396,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1744,479 +1744,479 @@
       <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7265625" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="35" max="37" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="40" max="42" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="43" max="44" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="45" max="47" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="50" max="52" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="55" max="56" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="58" max="59" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="61" max="62" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="63" max="64" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="65" max="67" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="68" max="69" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="70" max="72" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="73" max="74" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="75" max="76" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="78" max="79" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="80" max="82" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="83" max="84" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="85" max="87" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="88" max="89" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="90" max="92" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="93" max="94" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="95" max="97" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="98" max="99" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="100" max="102" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="103" max="104" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="105" max="107" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="108" max="109" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="110" max="112" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="113" max="114" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="116" max="117" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="118" max="119" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="121" max="122" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="123" max="124" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="125" max="127" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="128" max="129" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="130" max="132" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="37" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="42" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="52" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="56" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="58" max="59" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="62" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="67" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="68" max="69" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="70" max="72" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="73" max="74" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="75" max="76" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="78" max="79" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="80" max="82" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="83" max="84" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="85" max="87" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="88" max="89" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="90" max="92" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="93" max="94" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="95" max="97" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="98" max="99" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="100" max="102" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="103" max="104" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="105" max="107" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="108" max="109" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="110" max="112" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="113" max="114" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="116" max="117" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="118" max="119" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="121" max="122" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="123" max="124" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="125" max="127" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="128" max="129" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="130" max="132" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:132" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B1" s="40" t="s">
+    <row r="1" spans="1:132" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="43" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40"/>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="40"/>
-      <c r="Z1" s="40"/>
-      <c r="AA1" s="40"/>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="40"/>
-      <c r="AG1" s="40"/>
-      <c r="AH1" s="40"/>
-      <c r="AI1" s="40"/>
-      <c r="AJ1" s="40"/>
-      <c r="AK1" s="40"/>
-      <c r="AL1" s="40"/>
-      <c r="AM1" s="40"/>
-      <c r="AN1" s="40"/>
-      <c r="AO1" s="40"/>
-      <c r="AP1" s="40"/>
-      <c r="AQ1" s="40"/>
-      <c r="AR1" s="40"/>
-      <c r="AS1" s="40"/>
-      <c r="AT1" s="40"/>
-      <c r="AU1" s="40"/>
-      <c r="AV1" s="40"/>
-      <c r="AW1" s="40"/>
-      <c r="AX1" s="40"/>
-      <c r="AY1" s="40"/>
-      <c r="AZ1" s="40"/>
-      <c r="BA1" s="40"/>
-      <c r="BB1" s="40"/>
-      <c r="BC1" s="40"/>
-      <c r="BD1" s="40"/>
-      <c r="BE1" s="40"/>
-      <c r="BF1" s="40"/>
-      <c r="BG1" s="40"/>
-      <c r="BH1" s="40"/>
-      <c r="BI1" s="40"/>
-      <c r="BJ1" s="40"/>
-      <c r="BK1" s="40"/>
-      <c r="BL1" s="40"/>
-      <c r="BM1" s="40"/>
-      <c r="BN1" s="40"/>
-      <c r="BO1" s="40"/>
-      <c r="BP1" s="40"/>
-      <c r="BQ1" s="40"/>
-      <c r="BR1" s="40"/>
-      <c r="BS1" s="40"/>
-      <c r="BT1" s="40"/>
-      <c r="BU1" s="40"/>
-      <c r="BV1" s="40"/>
-      <c r="BW1" s="40"/>
-      <c r="BX1" s="40"/>
-      <c r="BY1" s="40"/>
-      <c r="BZ1" s="40"/>
-      <c r="CA1" s="40"/>
-      <c r="CB1" s="40"/>
-      <c r="CC1" s="40"/>
-      <c r="CD1" s="40"/>
-      <c r="CE1" s="40"/>
-      <c r="CF1" s="40"/>
-      <c r="CG1" s="40"/>
-      <c r="CH1" s="40"/>
-      <c r="CI1" s="40"/>
-      <c r="CJ1" s="40"/>
-      <c r="CK1" s="40"/>
-      <c r="CL1" s="40"/>
-      <c r="CM1" s="40"/>
-      <c r="CN1" s="40"/>
-      <c r="CO1" s="40"/>
-      <c r="CP1" s="40"/>
-      <c r="CQ1" s="40"/>
-      <c r="CR1" s="40"/>
-      <c r="CS1" s="40"/>
-      <c r="CT1" s="40"/>
-      <c r="CU1" s="40"/>
-      <c r="CV1" s="40"/>
-      <c r="CW1" s="40"/>
-      <c r="CX1" s="40"/>
-      <c r="CY1" s="40"/>
-      <c r="CZ1" s="40"/>
-      <c r="DA1" s="40"/>
-      <c r="DB1" s="40"/>
-      <c r="DC1" s="40"/>
-      <c r="DD1" s="40"/>
-      <c r="DE1" s="40"/>
-      <c r="DF1" s="40"/>
-      <c r="DG1" s="40"/>
-      <c r="DH1" s="40"/>
-      <c r="DI1" s="40"/>
-      <c r="DJ1" s="40"/>
-      <c r="DK1" s="40"/>
-      <c r="DL1" s="40"/>
-      <c r="DM1" s="40"/>
-      <c r="DN1" s="40"/>
-      <c r="DO1" s="40"/>
-      <c r="DP1" s="40"/>
-      <c r="DQ1" s="40"/>
-      <c r="DR1" s="40"/>
-      <c r="DS1" s="40"/>
-      <c r="DT1" s="40"/>
-      <c r="DU1" s="40"/>
-      <c r="DV1" s="40"/>
-      <c r="DW1" s="40"/>
-      <c r="DX1" s="40"/>
-      <c r="DY1" s="40"/>
-      <c r="DZ1" s="40"/>
-      <c r="EA1" s="40"/>
-      <c r="EB1" s="40"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="43"/>
+      <c r="AC1" s="43"/>
+      <c r="AD1" s="43"/>
+      <c r="AE1" s="43"/>
+      <c r="AF1" s="43"/>
+      <c r="AG1" s="43"/>
+      <c r="AH1" s="43"/>
+      <c r="AI1" s="43"/>
+      <c r="AJ1" s="43"/>
+      <c r="AK1" s="43"/>
+      <c r="AL1" s="43"/>
+      <c r="AM1" s="43"/>
+      <c r="AN1" s="43"/>
+      <c r="AO1" s="43"/>
+      <c r="AP1" s="43"/>
+      <c r="AQ1" s="43"/>
+      <c r="AR1" s="43"/>
+      <c r="AS1" s="43"/>
+      <c r="AT1" s="43"/>
+      <c r="AU1" s="43"/>
+      <c r="AV1" s="43"/>
+      <c r="AW1" s="43"/>
+      <c r="AX1" s="43"/>
+      <c r="AY1" s="43"/>
+      <c r="AZ1" s="43"/>
+      <c r="BA1" s="43"/>
+      <c r="BB1" s="43"/>
+      <c r="BC1" s="43"/>
+      <c r="BD1" s="43"/>
+      <c r="BE1" s="43"/>
+      <c r="BF1" s="43"/>
+      <c r="BG1" s="43"/>
+      <c r="BH1" s="43"/>
+      <c r="BI1" s="43"/>
+      <c r="BJ1" s="43"/>
+      <c r="BK1" s="43"/>
+      <c r="BL1" s="43"/>
+      <c r="BM1" s="43"/>
+      <c r="BN1" s="43"/>
+      <c r="BO1" s="43"/>
+      <c r="BP1" s="43"/>
+      <c r="BQ1" s="43"/>
+      <c r="BR1" s="43"/>
+      <c r="BS1" s="43"/>
+      <c r="BT1" s="43"/>
+      <c r="BU1" s="43"/>
+      <c r="BV1" s="43"/>
+      <c r="BW1" s="43"/>
+      <c r="BX1" s="43"/>
+      <c r="BY1" s="43"/>
+      <c r="BZ1" s="43"/>
+      <c r="CA1" s="43"/>
+      <c r="CB1" s="43"/>
+      <c r="CC1" s="43"/>
+      <c r="CD1" s="43"/>
+      <c r="CE1" s="43"/>
+      <c r="CF1" s="43"/>
+      <c r="CG1" s="43"/>
+      <c r="CH1" s="43"/>
+      <c r="CI1" s="43"/>
+      <c r="CJ1" s="43"/>
+      <c r="CK1" s="43"/>
+      <c r="CL1" s="43"/>
+      <c r="CM1" s="43"/>
+      <c r="CN1" s="43"/>
+      <c r="CO1" s="43"/>
+      <c r="CP1" s="43"/>
+      <c r="CQ1" s="43"/>
+      <c r="CR1" s="43"/>
+      <c r="CS1" s="43"/>
+      <c r="CT1" s="43"/>
+      <c r="CU1" s="43"/>
+      <c r="CV1" s="43"/>
+      <c r="CW1" s="43"/>
+      <c r="CX1" s="43"/>
+      <c r="CY1" s="43"/>
+      <c r="CZ1" s="43"/>
+      <c r="DA1" s="43"/>
+      <c r="DB1" s="43"/>
+      <c r="DC1" s="43"/>
+      <c r="DD1" s="43"/>
+      <c r="DE1" s="43"/>
+      <c r="DF1" s="43"/>
+      <c r="DG1" s="43"/>
+      <c r="DH1" s="43"/>
+      <c r="DI1" s="43"/>
+      <c r="DJ1" s="43"/>
+      <c r="DK1" s="43"/>
+      <c r="DL1" s="43"/>
+      <c r="DM1" s="43"/>
+      <c r="DN1" s="43"/>
+      <c r="DO1" s="43"/>
+      <c r="DP1" s="43"/>
+      <c r="DQ1" s="43"/>
+      <c r="DR1" s="43"/>
+      <c r="DS1" s="43"/>
+      <c r="DT1" s="43"/>
+      <c r="DU1" s="43"/>
+      <c r="DV1" s="43"/>
+      <c r="DW1" s="43"/>
+      <c r="DX1" s="43"/>
+      <c r="DY1" s="43"/>
+      <c r="DZ1" s="43"/>
+      <c r="EA1" s="43"/>
+      <c r="EB1" s="43"/>
     </row>
-    <row r="2" spans="1:132" s="3" customFormat="1" ht="10" x14ac:dyDescent="0.2">
-      <c r="B2" s="41" t="s">
+    <row r="2" spans="1:132" s="3" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="B2" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="41"/>
-      <c r="V2" s="41"/>
-      <c r="W2" s="41"/>
-      <c r="X2" s="41"/>
-      <c r="Y2" s="41"/>
-      <c r="Z2" s="41"/>
-      <c r="AA2" s="41"/>
-      <c r="AB2" s="41"/>
-      <c r="AC2" s="41"/>
-      <c r="AD2" s="41"/>
-      <c r="AE2" s="41"/>
-      <c r="AF2" s="41"/>
-      <c r="AG2" s="41"/>
-      <c r="AH2" s="41"/>
-      <c r="AI2" s="41"/>
-      <c r="AJ2" s="41"/>
-      <c r="AK2" s="41"/>
-      <c r="AL2" s="41"/>
-      <c r="AM2" s="41"/>
-      <c r="AN2" s="41"/>
-      <c r="AO2" s="41"/>
-      <c r="AP2" s="41"/>
-      <c r="AQ2" s="41"/>
-      <c r="AR2" s="41"/>
-      <c r="AS2" s="41"/>
-      <c r="AT2" s="41"/>
-      <c r="AU2" s="41"/>
-      <c r="AV2" s="41"/>
-      <c r="AW2" s="41"/>
-      <c r="AX2" s="41"/>
-      <c r="AY2" s="41"/>
-      <c r="AZ2" s="41"/>
-      <c r="BA2" s="41"/>
-      <c r="BB2" s="41"/>
-      <c r="BC2" s="41"/>
-      <c r="BD2" s="41"/>
-      <c r="BE2" s="41"/>
-      <c r="BF2" s="41"/>
-      <c r="BG2" s="41"/>
-      <c r="BH2" s="41"/>
-      <c r="BI2" s="41"/>
-      <c r="BJ2" s="41"/>
-      <c r="BK2" s="41"/>
-      <c r="BL2" s="41"/>
-      <c r="BM2" s="41"/>
-      <c r="BN2" s="41"/>
-      <c r="BO2" s="41"/>
-      <c r="BP2" s="41"/>
-      <c r="BQ2" s="41"/>
-      <c r="BR2" s="41"/>
-      <c r="BS2" s="41"/>
-      <c r="BT2" s="41"/>
-      <c r="BU2" s="41"/>
-      <c r="BV2" s="41"/>
-      <c r="BW2" s="41"/>
-      <c r="BX2" s="41"/>
-      <c r="BY2" s="41"/>
-      <c r="BZ2" s="41"/>
-      <c r="CA2" s="41"/>
-      <c r="CB2" s="41"/>
-      <c r="CC2" s="41"/>
-      <c r="CD2" s="41"/>
-      <c r="CE2" s="41"/>
-      <c r="CF2" s="41"/>
-      <c r="CG2" s="41"/>
-      <c r="CH2" s="41"/>
-      <c r="CI2" s="41"/>
-      <c r="CJ2" s="41"/>
-      <c r="CK2" s="41"/>
-      <c r="CL2" s="41"/>
-      <c r="CM2" s="41"/>
-      <c r="CN2" s="41"/>
-      <c r="CO2" s="41"/>
-      <c r="CP2" s="41"/>
-      <c r="CQ2" s="41"/>
-      <c r="CR2" s="41"/>
-      <c r="CS2" s="41"/>
-      <c r="CT2" s="41"/>
-      <c r="CU2" s="41"/>
-      <c r="CV2" s="41"/>
-      <c r="CW2" s="41"/>
-      <c r="CX2" s="41"/>
-      <c r="CY2" s="41"/>
-      <c r="CZ2" s="41"/>
-      <c r="DA2" s="41"/>
-      <c r="DB2" s="41"/>
-      <c r="DC2" s="41"/>
-      <c r="DD2" s="41"/>
-      <c r="DE2" s="41"/>
-      <c r="DF2" s="41"/>
-      <c r="DG2" s="41"/>
-      <c r="DH2" s="41"/>
-      <c r="DI2" s="41"/>
-      <c r="DJ2" s="41"/>
-      <c r="DK2" s="41"/>
-      <c r="DL2" s="41"/>
-      <c r="DM2" s="41"/>
-      <c r="DN2" s="41"/>
-      <c r="DO2" s="41"/>
-      <c r="DP2" s="41"/>
-      <c r="DQ2" s="41"/>
-      <c r="DR2" s="41"/>
-      <c r="DS2" s="41"/>
-      <c r="DT2" s="41"/>
-      <c r="DU2" s="41"/>
-      <c r="DV2" s="41"/>
-      <c r="DW2" s="41"/>
-      <c r="DX2" s="41"/>
-      <c r="DY2" s="41"/>
-      <c r="DZ2" s="41"/>
-      <c r="EA2" s="41"/>
-      <c r="EB2" s="41"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
+      <c r="V2" s="44"/>
+      <c r="W2" s="44"/>
+      <c r="X2" s="44"/>
+      <c r="Y2" s="44"/>
+      <c r="Z2" s="44"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
+      <c r="AF2" s="44"/>
+      <c r="AG2" s="44"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="44"/>
+      <c r="AL2" s="44"/>
+      <c r="AM2" s="44"/>
+      <c r="AN2" s="44"/>
+      <c r="AO2" s="44"/>
+      <c r="AP2" s="44"/>
+      <c r="AQ2" s="44"/>
+      <c r="AR2" s="44"/>
+      <c r="AS2" s="44"/>
+      <c r="AT2" s="44"/>
+      <c r="AU2" s="44"/>
+      <c r="AV2" s="44"/>
+      <c r="AW2" s="44"/>
+      <c r="AX2" s="44"/>
+      <c r="AY2" s="44"/>
+      <c r="AZ2" s="44"/>
+      <c r="BA2" s="44"/>
+      <c r="BB2" s="44"/>
+      <c r="BC2" s="44"/>
+      <c r="BD2" s="44"/>
+      <c r="BE2" s="44"/>
+      <c r="BF2" s="44"/>
+      <c r="BG2" s="44"/>
+      <c r="BH2" s="44"/>
+      <c r="BI2" s="44"/>
+      <c r="BJ2" s="44"/>
+      <c r="BK2" s="44"/>
+      <c r="BL2" s="44"/>
+      <c r="BM2" s="44"/>
+      <c r="BN2" s="44"/>
+      <c r="BO2" s="44"/>
+      <c r="BP2" s="44"/>
+      <c r="BQ2" s="44"/>
+      <c r="BR2" s="44"/>
+      <c r="BS2" s="44"/>
+      <c r="BT2" s="44"/>
+      <c r="BU2" s="44"/>
+      <c r="BV2" s="44"/>
+      <c r="BW2" s="44"/>
+      <c r="BX2" s="44"/>
+      <c r="BY2" s="44"/>
+      <c r="BZ2" s="44"/>
+      <c r="CA2" s="44"/>
+      <c r="CB2" s="44"/>
+      <c r="CC2" s="44"/>
+      <c r="CD2" s="44"/>
+      <c r="CE2" s="44"/>
+      <c r="CF2" s="44"/>
+      <c r="CG2" s="44"/>
+      <c r="CH2" s="44"/>
+      <c r="CI2" s="44"/>
+      <c r="CJ2" s="44"/>
+      <c r="CK2" s="44"/>
+      <c r="CL2" s="44"/>
+      <c r="CM2" s="44"/>
+      <c r="CN2" s="44"/>
+      <c r="CO2" s="44"/>
+      <c r="CP2" s="44"/>
+      <c r="CQ2" s="44"/>
+      <c r="CR2" s="44"/>
+      <c r="CS2" s="44"/>
+      <c r="CT2" s="44"/>
+      <c r="CU2" s="44"/>
+      <c r="CV2" s="44"/>
+      <c r="CW2" s="44"/>
+      <c r="CX2" s="44"/>
+      <c r="CY2" s="44"/>
+      <c r="CZ2" s="44"/>
+      <c r="DA2" s="44"/>
+      <c r="DB2" s="44"/>
+      <c r="DC2" s="44"/>
+      <c r="DD2" s="44"/>
+      <c r="DE2" s="44"/>
+      <c r="DF2" s="44"/>
+      <c r="DG2" s="44"/>
+      <c r="DH2" s="44"/>
+      <c r="DI2" s="44"/>
+      <c r="DJ2" s="44"/>
+      <c r="DK2" s="44"/>
+      <c r="DL2" s="44"/>
+      <c r="DM2" s="44"/>
+      <c r="DN2" s="44"/>
+      <c r="DO2" s="44"/>
+      <c r="DP2" s="44"/>
+      <c r="DQ2" s="44"/>
+      <c r="DR2" s="44"/>
+      <c r="DS2" s="44"/>
+      <c r="DT2" s="44"/>
+      <c r="DU2" s="44"/>
+      <c r="DV2" s="44"/>
+      <c r="DW2" s="44"/>
+      <c r="DX2" s="44"/>
+      <c r="DY2" s="44"/>
+      <c r="DZ2" s="44"/>
+      <c r="EA2" s="44"/>
+      <c r="EB2" s="44"/>
     </row>
-    <row r="3" spans="1:132" s="3" customFormat="1" ht="10" x14ac:dyDescent="0.2">
-      <c r="B3" s="41" t="s">
+    <row r="3" spans="1:132" s="3" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="B3" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
-      <c r="T3" s="41"/>
-      <c r="U3" s="41"/>
-      <c r="V3" s="41"/>
-      <c r="W3" s="41"/>
-      <c r="X3" s="41"/>
-      <c r="Y3" s="41"/>
-      <c r="Z3" s="41"/>
-      <c r="AA3" s="41"/>
-      <c r="AB3" s="41"/>
-      <c r="AC3" s="41"/>
-      <c r="AD3" s="41"/>
-      <c r="AE3" s="41"/>
-      <c r="AF3" s="41"/>
-      <c r="AG3" s="41"/>
-      <c r="AH3" s="41"/>
-      <c r="AI3" s="41"/>
-      <c r="AJ3" s="41"/>
-      <c r="AK3" s="41"/>
-      <c r="AL3" s="41"/>
-      <c r="AM3" s="41"/>
-      <c r="AN3" s="41"/>
-      <c r="AO3" s="41"/>
-      <c r="AP3" s="41"/>
-      <c r="AQ3" s="41"/>
-      <c r="AR3" s="41"/>
-      <c r="AS3" s="41"/>
-      <c r="AT3" s="41"/>
-      <c r="AU3" s="41"/>
-      <c r="AV3" s="41"/>
-      <c r="AW3" s="41"/>
-      <c r="AX3" s="41"/>
-      <c r="AY3" s="41"/>
-      <c r="AZ3" s="41"/>
-      <c r="BA3" s="41"/>
-      <c r="BB3" s="41"/>
-      <c r="BC3" s="41"/>
-      <c r="BD3" s="41"/>
-      <c r="BE3" s="41"/>
-      <c r="BF3" s="41"/>
-      <c r="BG3" s="41"/>
-      <c r="BH3" s="41"/>
-      <c r="BI3" s="41"/>
-      <c r="BJ3" s="41"/>
-      <c r="BK3" s="41"/>
-      <c r="BL3" s="41"/>
-      <c r="BM3" s="41"/>
-      <c r="BN3" s="41"/>
-      <c r="BO3" s="41"/>
-      <c r="BP3" s="41"/>
-      <c r="BQ3" s="41"/>
-      <c r="BR3" s="41"/>
-      <c r="BS3" s="41"/>
-      <c r="BT3" s="41"/>
-      <c r="BU3" s="41"/>
-      <c r="BV3" s="41"/>
-      <c r="BW3" s="41"/>
-      <c r="BX3" s="41"/>
-      <c r="BY3" s="41"/>
-      <c r="BZ3" s="41"/>
-      <c r="CA3" s="41"/>
-      <c r="CB3" s="41"/>
-      <c r="CC3" s="41"/>
-      <c r="CD3" s="41"/>
-      <c r="CE3" s="41"/>
-      <c r="CF3" s="41"/>
-      <c r="CG3" s="41"/>
-      <c r="CH3" s="41"/>
-      <c r="CI3" s="41"/>
-      <c r="CJ3" s="41"/>
-      <c r="CK3" s="41"/>
-      <c r="CL3" s="41"/>
-      <c r="CM3" s="41"/>
-      <c r="CN3" s="41"/>
-      <c r="CO3" s="41"/>
-      <c r="CP3" s="41"/>
-      <c r="CQ3" s="41"/>
-      <c r="CR3" s="41"/>
-      <c r="CS3" s="41"/>
-      <c r="CT3" s="41"/>
-      <c r="CU3" s="41"/>
-      <c r="CV3" s="41"/>
-      <c r="CW3" s="41"/>
-      <c r="CX3" s="41"/>
-      <c r="CY3" s="41"/>
-      <c r="CZ3" s="41"/>
-      <c r="DA3" s="41"/>
-      <c r="DB3" s="41"/>
-      <c r="DC3" s="41"/>
-      <c r="DD3" s="41"/>
-      <c r="DE3" s="41"/>
-      <c r="DF3" s="41"/>
-      <c r="DG3" s="41"/>
-      <c r="DH3" s="41"/>
-      <c r="DI3" s="41"/>
-      <c r="DJ3" s="41"/>
-      <c r="DK3" s="41"/>
-      <c r="DL3" s="41"/>
-      <c r="DM3" s="41"/>
-      <c r="DN3" s="41"/>
-      <c r="DO3" s="41"/>
-      <c r="DP3" s="41"/>
-      <c r="DQ3" s="41"/>
-      <c r="DR3" s="41"/>
-      <c r="DS3" s="41"/>
-      <c r="DT3" s="41"/>
-      <c r="DU3" s="41"/>
-      <c r="DV3" s="41"/>
-      <c r="DW3" s="41"/>
-      <c r="DX3" s="41"/>
-      <c r="DY3" s="41"/>
-      <c r="DZ3" s="41"/>
-      <c r="EA3" s="41"/>
-      <c r="EB3" s="41"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
+      <c r="U3" s="44"/>
+      <c r="V3" s="44"/>
+      <c r="W3" s="44"/>
+      <c r="X3" s="44"/>
+      <c r="Y3" s="44"/>
+      <c r="Z3" s="44"/>
+      <c r="AA3" s="44"/>
+      <c r="AB3" s="44"/>
+      <c r="AC3" s="44"/>
+      <c r="AD3" s="44"/>
+      <c r="AE3" s="44"/>
+      <c r="AF3" s="44"/>
+      <c r="AG3" s="44"/>
+      <c r="AH3" s="44"/>
+      <c r="AI3" s="44"/>
+      <c r="AJ3" s="44"/>
+      <c r="AK3" s="44"/>
+      <c r="AL3" s="44"/>
+      <c r="AM3" s="44"/>
+      <c r="AN3" s="44"/>
+      <c r="AO3" s="44"/>
+      <c r="AP3" s="44"/>
+      <c r="AQ3" s="44"/>
+      <c r="AR3" s="44"/>
+      <c r="AS3" s="44"/>
+      <c r="AT3" s="44"/>
+      <c r="AU3" s="44"/>
+      <c r="AV3" s="44"/>
+      <c r="AW3" s="44"/>
+      <c r="AX3" s="44"/>
+      <c r="AY3" s="44"/>
+      <c r="AZ3" s="44"/>
+      <c r="BA3" s="44"/>
+      <c r="BB3" s="44"/>
+      <c r="BC3" s="44"/>
+      <c r="BD3" s="44"/>
+      <c r="BE3" s="44"/>
+      <c r="BF3" s="44"/>
+      <c r="BG3" s="44"/>
+      <c r="BH3" s="44"/>
+      <c r="BI3" s="44"/>
+      <c r="BJ3" s="44"/>
+      <c r="BK3" s="44"/>
+      <c r="BL3" s="44"/>
+      <c r="BM3" s="44"/>
+      <c r="BN3" s="44"/>
+      <c r="BO3" s="44"/>
+      <c r="BP3" s="44"/>
+      <c r="BQ3" s="44"/>
+      <c r="BR3" s="44"/>
+      <c r="BS3" s="44"/>
+      <c r="BT3" s="44"/>
+      <c r="BU3" s="44"/>
+      <c r="BV3" s="44"/>
+      <c r="BW3" s="44"/>
+      <c r="BX3" s="44"/>
+      <c r="BY3" s="44"/>
+      <c r="BZ3" s="44"/>
+      <c r="CA3" s="44"/>
+      <c r="CB3" s="44"/>
+      <c r="CC3" s="44"/>
+      <c r="CD3" s="44"/>
+      <c r="CE3" s="44"/>
+      <c r="CF3" s="44"/>
+      <c r="CG3" s="44"/>
+      <c r="CH3" s="44"/>
+      <c r="CI3" s="44"/>
+      <c r="CJ3" s="44"/>
+      <c r="CK3" s="44"/>
+      <c r="CL3" s="44"/>
+      <c r="CM3" s="44"/>
+      <c r="CN3" s="44"/>
+      <c r="CO3" s="44"/>
+      <c r="CP3" s="44"/>
+      <c r="CQ3" s="44"/>
+      <c r="CR3" s="44"/>
+      <c r="CS3" s="44"/>
+      <c r="CT3" s="44"/>
+      <c r="CU3" s="44"/>
+      <c r="CV3" s="44"/>
+      <c r="CW3" s="44"/>
+      <c r="CX3" s="44"/>
+      <c r="CY3" s="44"/>
+      <c r="CZ3" s="44"/>
+      <c r="DA3" s="44"/>
+      <c r="DB3" s="44"/>
+      <c r="DC3" s="44"/>
+      <c r="DD3" s="44"/>
+      <c r="DE3" s="44"/>
+      <c r="DF3" s="44"/>
+      <c r="DG3" s="44"/>
+      <c r="DH3" s="44"/>
+      <c r="DI3" s="44"/>
+      <c r="DJ3" s="44"/>
+      <c r="DK3" s="44"/>
+      <c r="DL3" s="44"/>
+      <c r="DM3" s="44"/>
+      <c r="DN3" s="44"/>
+      <c r="DO3" s="44"/>
+      <c r="DP3" s="44"/>
+      <c r="DQ3" s="44"/>
+      <c r="DR3" s="44"/>
+      <c r="DS3" s="44"/>
+      <c r="DT3" s="44"/>
+      <c r="DU3" s="44"/>
+      <c r="DV3" s="44"/>
+      <c r="DW3" s="44"/>
+      <c r="DX3" s="44"/>
+      <c r="DY3" s="44"/>
+      <c r="DZ3" s="44"/>
+      <c r="EA3" s="44"/>
+      <c r="EB3" s="44"/>
     </row>
-    <row r="4" spans="1:132" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:132" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>186</v>
       </c>
@@ -2351,7 +2351,7 @@
       <c r="EA4" s="6"/>
       <c r="EB4" s="7"/>
     </row>
-    <row r="5" spans="1:132" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:132" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>148</v>
       </c>
@@ -2486,7 +2486,7 @@
       <c r="EA5" s="6"/>
       <c r="EB5" s="7"/>
     </row>
-    <row r="6" spans="1:132" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:132" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>187</v>
       </c>
@@ -2621,7 +2621,7 @@
       <c r="EA6" s="6"/>
       <c r="EB6" s="7"/>
     </row>
-    <row r="7" spans="1:132" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:132" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>149</v>
       </c>
@@ -2756,7 +2756,7 @@
       <c r="EA7" s="6"/>
       <c r="EB7" s="7"/>
     </row>
-    <row r="8" spans="1:132" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:132" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>150</v>
       </c>
@@ -2891,22 +2891,22 @@
       <c r="EA8" s="6"/>
       <c r="EB8" s="7"/>
     </row>
-    <row r="9" spans="1:132" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="42" t="s">
+    <row r="9" spans="1:132" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="C9" s="42"/>
+      <c r="C9" s="45"/>
       <c r="D9" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="46" t="s">
         <v>189</v>
       </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
       <c r="K9" s="10"/>
       <c r="L9" s="7"/>
       <c r="M9" s="6"/>
@@ -3030,195 +3030,195 @@
       <c r="EA9" s="6"/>
       <c r="EB9" s="7"/>
     </row>
-    <row r="10" spans="1:132" s="11" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="44" t="s">
+    <row r="10" spans="1:132" s="11" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="37" t="s">
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="34" t="s">
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="37" t="s">
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="39"/>
+      <c r="R10" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="S10" s="38"/>
-      <c r="T10" s="38"/>
-      <c r="U10" s="38"/>
-      <c r="V10" s="39"/>
-      <c r="W10" s="34" t="s">
+      <c r="S10" s="41"/>
+      <c r="T10" s="41"/>
+      <c r="U10" s="41"/>
+      <c r="V10" s="42"/>
+      <c r="W10" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="X10" s="35"/>
-      <c r="Y10" s="35"/>
-      <c r="Z10" s="35"/>
-      <c r="AA10" s="36"/>
-      <c r="AB10" s="37" t="s">
+      <c r="X10" s="38"/>
+      <c r="Y10" s="38"/>
+      <c r="Z10" s="38"/>
+      <c r="AA10" s="39"/>
+      <c r="AB10" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="AC10" s="38"/>
-      <c r="AD10" s="38"/>
-      <c r="AE10" s="38"/>
-      <c r="AF10" s="39"/>
-      <c r="AG10" s="34" t="s">
+      <c r="AC10" s="41"/>
+      <c r="AD10" s="41"/>
+      <c r="AE10" s="41"/>
+      <c r="AF10" s="42"/>
+      <c r="AG10" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="AH10" s="35"/>
-      <c r="AI10" s="35"/>
-      <c r="AJ10" s="35"/>
-      <c r="AK10" s="36"/>
-      <c r="AL10" s="37" t="s">
+      <c r="AH10" s="38"/>
+      <c r="AI10" s="38"/>
+      <c r="AJ10" s="38"/>
+      <c r="AK10" s="39"/>
+      <c r="AL10" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="AM10" s="38"/>
-      <c r="AN10" s="38"/>
-      <c r="AO10" s="38"/>
-      <c r="AP10" s="39"/>
-      <c r="AQ10" s="34" t="s">
+      <c r="AM10" s="41"/>
+      <c r="AN10" s="41"/>
+      <c r="AO10" s="41"/>
+      <c r="AP10" s="42"/>
+      <c r="AQ10" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="AR10" s="35"/>
-      <c r="AS10" s="35"/>
-      <c r="AT10" s="35"/>
-      <c r="AU10" s="36"/>
-      <c r="AV10" s="37" t="s">
+      <c r="AR10" s="38"/>
+      <c r="AS10" s="38"/>
+      <c r="AT10" s="38"/>
+      <c r="AU10" s="39"/>
+      <c r="AV10" s="40" t="s">
         <v>161</v>
       </c>
-      <c r="AW10" s="38"/>
-      <c r="AX10" s="38"/>
-      <c r="AY10" s="38"/>
-      <c r="AZ10" s="39"/>
-      <c r="BA10" s="34" t="s">
+      <c r="AW10" s="41"/>
+      <c r="AX10" s="41"/>
+      <c r="AY10" s="41"/>
+      <c r="AZ10" s="42"/>
+      <c r="BA10" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="BB10" s="35"/>
-      <c r="BC10" s="35"/>
-      <c r="BD10" s="35"/>
-      <c r="BE10" s="36"/>
-      <c r="BF10" s="34" t="s">
+      <c r="BB10" s="38"/>
+      <c r="BC10" s="38"/>
+      <c r="BD10" s="38"/>
+      <c r="BE10" s="39"/>
+      <c r="BF10" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="BG10" s="35"/>
-      <c r="BH10" s="35"/>
-      <c r="BI10" s="35"/>
-      <c r="BJ10" s="36"/>
-      <c r="BK10" s="34" t="s">
+      <c r="BG10" s="38"/>
+      <c r="BH10" s="38"/>
+      <c r="BI10" s="38"/>
+      <c r="BJ10" s="39"/>
+      <c r="BK10" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="BL10" s="35"/>
-      <c r="BM10" s="35"/>
-      <c r="BN10" s="35"/>
-      <c r="BO10" s="36"/>
-      <c r="BP10" s="34" t="s">
+      <c r="BL10" s="38"/>
+      <c r="BM10" s="38"/>
+      <c r="BN10" s="38"/>
+      <c r="BO10" s="39"/>
+      <c r="BP10" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="BQ10" s="35"/>
-      <c r="BR10" s="35"/>
-      <c r="BS10" s="35"/>
-      <c r="BT10" s="36"/>
-      <c r="BU10" s="34" t="s">
+      <c r="BQ10" s="38"/>
+      <c r="BR10" s="38"/>
+      <c r="BS10" s="38"/>
+      <c r="BT10" s="39"/>
+      <c r="BU10" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="BV10" s="35"/>
-      <c r="BW10" s="35"/>
-      <c r="BX10" s="35"/>
-      <c r="BY10" s="36"/>
-      <c r="BZ10" s="34" t="s">
+      <c r="BV10" s="38"/>
+      <c r="BW10" s="38"/>
+      <c r="BX10" s="38"/>
+      <c r="BY10" s="39"/>
+      <c r="BZ10" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="CA10" s="35"/>
-      <c r="CB10" s="35"/>
-      <c r="CC10" s="35"/>
-      <c r="CD10" s="36"/>
-      <c r="CE10" s="34" t="s">
+      <c r="CA10" s="38"/>
+      <c r="CB10" s="38"/>
+      <c r="CC10" s="38"/>
+      <c r="CD10" s="39"/>
+      <c r="CE10" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="CF10" s="35"/>
-      <c r="CG10" s="35"/>
-      <c r="CH10" s="35"/>
-      <c r="CI10" s="36"/>
-      <c r="CJ10" s="34" t="s">
+      <c r="CF10" s="38"/>
+      <c r="CG10" s="38"/>
+      <c r="CH10" s="38"/>
+      <c r="CI10" s="39"/>
+      <c r="CJ10" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="CK10" s="35"/>
-      <c r="CL10" s="35"/>
-      <c r="CM10" s="35"/>
-      <c r="CN10" s="36"/>
-      <c r="CO10" s="34" t="s">
+      <c r="CK10" s="38"/>
+      <c r="CL10" s="38"/>
+      <c r="CM10" s="38"/>
+      <c r="CN10" s="39"/>
+      <c r="CO10" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="CP10" s="35"/>
-      <c r="CQ10" s="35"/>
-      <c r="CR10" s="35"/>
-      <c r="CS10" s="36"/>
-      <c r="CT10" s="34" t="s">
+      <c r="CP10" s="38"/>
+      <c r="CQ10" s="38"/>
+      <c r="CR10" s="38"/>
+      <c r="CS10" s="39"/>
+      <c r="CT10" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="CU10" s="35"/>
-      <c r="CV10" s="35"/>
-      <c r="CW10" s="35"/>
-      <c r="CX10" s="36"/>
-      <c r="CY10" s="34" t="s">
+      <c r="CU10" s="38"/>
+      <c r="CV10" s="38"/>
+      <c r="CW10" s="38"/>
+      <c r="CX10" s="39"/>
+      <c r="CY10" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="CZ10" s="35"/>
-      <c r="DA10" s="35"/>
-      <c r="DB10" s="35"/>
-      <c r="DC10" s="36"/>
-      <c r="DD10" s="34" t="s">
+      <c r="CZ10" s="38"/>
+      <c r="DA10" s="38"/>
+      <c r="DB10" s="38"/>
+      <c r="DC10" s="39"/>
+      <c r="DD10" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="DE10" s="35"/>
-      <c r="DF10" s="35"/>
-      <c r="DG10" s="35"/>
-      <c r="DH10" s="36"/>
-      <c r="DI10" s="34" t="s">
+      <c r="DE10" s="38"/>
+      <c r="DF10" s="38"/>
+      <c r="DG10" s="38"/>
+      <c r="DH10" s="39"/>
+      <c r="DI10" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="DJ10" s="35"/>
-      <c r="DK10" s="35"/>
-      <c r="DL10" s="35"/>
-      <c r="DM10" s="36"/>
-      <c r="DN10" s="34" t="s">
+      <c r="DJ10" s="38"/>
+      <c r="DK10" s="38"/>
+      <c r="DL10" s="38"/>
+      <c r="DM10" s="39"/>
+      <c r="DN10" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="DO10" s="35"/>
-      <c r="DP10" s="35"/>
-      <c r="DQ10" s="35"/>
-      <c r="DR10" s="36"/>
-      <c r="DS10" s="34" t="s">
+      <c r="DO10" s="38"/>
+      <c r="DP10" s="38"/>
+      <c r="DQ10" s="38"/>
+      <c r="DR10" s="39"/>
+      <c r="DS10" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="DT10" s="35"/>
-      <c r="DU10" s="35"/>
-      <c r="DV10" s="35"/>
-      <c r="DW10" s="36"/>
-      <c r="DX10" s="34" t="s">
+      <c r="DT10" s="38"/>
+      <c r="DU10" s="38"/>
+      <c r="DV10" s="38"/>
+      <c r="DW10" s="39"/>
+      <c r="DX10" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="DY10" s="35"/>
-      <c r="DZ10" s="35"/>
-      <c r="EA10" s="35"/>
-      <c r="EB10" s="35"/>
+      <c r="DY10" s="38"/>
+      <c r="DZ10" s="38"/>
+      <c r="EA10" s="38"/>
+      <c r="EB10" s="38"/>
     </row>
-    <row r="11" spans="1:132" s="11" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="45"/>
+    <row r="11" spans="1:132" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B11" s="35"/>
       <c r="C11" s="12" t="s">
         <v>178</v>
       </c>
@@ -3610,8 +3610,8 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:132" s="11" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="45"/>
+    <row r="12" spans="1:132" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B12" s="35"/>
       <c r="C12" s="15" t="s">
         <v>181</v>
       </c>
@@ -4003,8 +4003,8 @@
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:132" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="45"/>
+    <row r="13" spans="1:132" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B13" s="35"/>
       <c r="C13" s="18" t="s">
         <v>182</v>
       </c>
@@ -4396,8 +4396,8 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:132" s="20" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="46"/>
+    <row r="14" spans="1:132" s="20" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="36"/>
       <c r="C14" s="21">
         <v>1</v>
       </c>
@@ -4789,7 +4789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:132" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:132" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>0</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -5585,7 +5585,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="18" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -5983,7 +5983,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -6381,7 +6381,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="21" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -6779,7 +6779,7 @@
         <v>3.87</v>
       </c>
     </row>
-    <row r="22" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5</v>
       </c>
@@ -7177,7 +7177,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="23" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6</v>
       </c>
@@ -7575,7 +7575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>7</v>
       </c>
@@ -7973,7 +7973,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>8</v>
       </c>
@@ -8371,7 +8371,7 @@
         <v>2.2400000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>9</v>
       </c>
@@ -8769,7 +8769,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="28" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10</v>
       </c>
@@ -9167,7 +9167,7 @@
         <v>3.28</v>
       </c>
     </row>
-    <row r="29" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>11</v>
       </c>
@@ -9565,7 +9565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>12</v>
       </c>
@@ -9963,7 +9963,7 @@
         <v>3.28</v>
       </c>
     </row>
-    <row r="31" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>13</v>
       </c>
@@ -10361,7 +10361,7 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>14</v>
       </c>
@@ -10759,7 +10759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>15</v>
       </c>
@@ -11157,7 +11157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>16</v>
       </c>
@@ -11555,7 +11555,7 @@
         <v>6.09</v>
       </c>
     </row>
-    <row r="35" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>17</v>
       </c>
@@ -11953,7 +11953,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="36" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>18</v>
       </c>
@@ -12351,7 +12351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>19</v>
       </c>
@@ -12749,7 +12749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>20</v>
       </c>
@@ -13147,7 +13147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>21</v>
       </c>
@@ -13545,7 +13545,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="41" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>22</v>
       </c>
@@ -13943,7 +13943,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="42" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>23</v>
       </c>
@@ -14341,7 +14341,7 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>24</v>
       </c>
@@ -14739,7 +14739,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="44" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>25</v>
       </c>
@@ -15137,7 +15137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>26</v>
       </c>
@@ -15535,7 +15535,7 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>27</v>
       </c>
@@ -15933,7 +15933,7 @@
         <v>1.18</v>
       </c>
     </row>
-    <row r="47" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>28</v>
       </c>
@@ -16331,7 +16331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>29</v>
       </c>
@@ -16729,7 +16729,7 @@
         <v>8.52</v>
       </c>
     </row>
-    <row r="49" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>30</v>
       </c>
@@ -17127,7 +17127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>31</v>
       </c>
@@ -17525,7 +17525,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="51" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>32</v>
       </c>
@@ -17923,7 +17923,7 @@
         <v>49.13</v>
       </c>
     </row>
-    <row r="52" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>33</v>
       </c>
@@ -18321,7 +18321,7 @@
         <v>4.66</v>
       </c>
     </row>
-    <row r="53" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>34</v>
       </c>
@@ -18719,7 +18719,7 @@
         <v>22.12</v>
       </c>
     </row>
-    <row r="54" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>35</v>
       </c>
@@ -19117,7 +19117,7 @@
         <v>5.87</v>
       </c>
     </row>
-    <row r="55" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>36</v>
       </c>
@@ -19515,7 +19515,7 @@
         <v>9.14</v>
       </c>
     </row>
-    <row r="56" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>37</v>
       </c>
@@ -19913,7 +19913,7 @@
         <v>6.94</v>
       </c>
     </row>
-    <row r="58" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>38</v>
       </c>
@@ -20311,7 +20311,7 @@
         <v>2.63</v>
       </c>
     </row>
-    <row r="59" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>39</v>
       </c>
@@ -20709,7 +20709,7 @@
         <v>3.26</v>
       </c>
     </row>
-    <row r="60" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>40</v>
       </c>
@@ -21107,7 +21107,7 @@
         <v>18.309999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>41</v>
       </c>
@@ -21505,7 +21505,7 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="62" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>42</v>
       </c>
@@ -21903,7 +21903,7 @@
         <v>3.57</v>
       </c>
     </row>
-    <row r="64" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>43</v>
       </c>
@@ -22301,7 +22301,7 @@
         <v>3.27</v>
       </c>
     </row>
-    <row r="65" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>44</v>
       </c>
@@ -22699,7 +22699,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="66" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>45</v>
       </c>
@@ -23097,7 +23097,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="67" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>46</v>
       </c>
@@ -23495,7 +23495,7 @@
         <v>9.18</v>
       </c>
     </row>
-    <row r="68" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>47</v>
       </c>
@@ -23893,7 +23893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>48</v>
       </c>
@@ -24291,7 +24291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>49</v>
       </c>
@@ -24689,7 +24689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>50</v>
       </c>
@@ -25087,7 +25087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>51</v>
       </c>
@@ -25485,7 +25485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>52</v>
       </c>
@@ -25883,7 +25883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>53</v>
       </c>
@@ -26281,7 +26281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>54</v>
       </c>
@@ -26679,12 +26679,12 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="80" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:132" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="81" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>55</v>
       </c>
@@ -27082,7 +27082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>56</v>
       </c>
@@ -27480,7 +27480,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="83" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>57</v>
       </c>
@@ -27878,7 +27878,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="84" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>58</v>
       </c>
@@ -28276,7 +28276,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="85" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>59</v>
       </c>
@@ -28674,7 +28674,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="86" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>60</v>
       </c>
@@ -29072,7 +29072,7 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>61</v>
       </c>
@@ -29470,7 +29470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>62</v>
       </c>
@@ -29868,7 +29868,7 @@
         <v>1.94</v>
       </c>
     </row>
-    <row r="89" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>63</v>
       </c>
@@ -30266,7 +30266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>64</v>
       </c>
@@ -30664,7 +30664,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="92" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>65</v>
       </c>
@@ -31062,7 +31062,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="93" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>66</v>
       </c>
@@ -31460,7 +31460,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="94" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>67</v>
       </c>
@@ -31858,7 +31858,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="95" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>68</v>
       </c>
@@ -32256,12 +32256,12 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="97" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:132" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="98" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>69</v>
       </c>
@@ -32659,7 +32659,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="99" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>70</v>
       </c>
@@ -33057,7 +33057,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="100" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>71</v>
       </c>
@@ -33455,7 +33455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>72</v>
       </c>
@@ -33853,7 +33853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>73</v>
       </c>
@@ -34251,7 +34251,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="103" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>74</v>
       </c>
@@ -34649,7 +34649,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="104" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>75</v>
       </c>
@@ -35047,7 +35047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>76</v>
       </c>
@@ -35445,12 +35445,12 @@
         <v>25.17</v>
       </c>
     </row>
-    <row r="107" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:132" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="108" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>77</v>
       </c>
@@ -35848,7 +35848,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="109" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>78</v>
       </c>
@@ -36246,7 +36246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>79</v>
       </c>
@@ -36644,7 +36644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>80</v>
       </c>
@@ -37042,7 +37042,7 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="112" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>81</v>
       </c>
@@ -37440,7 +37440,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="113" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>82</v>
       </c>
@@ -37838,7 +37838,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="114" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>83</v>
       </c>
@@ -38236,7 +38236,7 @@
         <v>6.32</v>
       </c>
     </row>
-    <row r="115" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>84</v>
       </c>
@@ -38634,7 +38634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>85</v>
       </c>
@@ -39032,12 +39032,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:132" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="119" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>86</v>
       </c>
@@ -39435,7 +39435,7 @@
         <v>4.37</v>
       </c>
     </row>
-    <row r="120" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>87</v>
       </c>
@@ -39833,7 +39833,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="121" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>88</v>
       </c>
@@ -40231,7 +40231,7 @@
         <v>8.82</v>
       </c>
     </row>
-    <row r="122" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>89</v>
       </c>
@@ -40629,7 +40629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>90</v>
       </c>
@@ -41027,12 +41027,12 @@
         <v>4.92</v>
       </c>
     </row>
-    <row r="125" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:132" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="126" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>92</v>
       </c>
@@ -41430,7 +41430,7 @@
         <v>4.83</v>
       </c>
     </row>
-    <row r="127" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>93</v>
       </c>
@@ -41828,7 +41828,7 @@
         <v>2.83</v>
       </c>
     </row>
-    <row r="128" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>94</v>
       </c>
@@ -42226,7 +42226,7 @@
         <v>5.94</v>
       </c>
     </row>
-    <row r="129" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>95</v>
       </c>
@@ -42624,7 +42624,7 @@
         <v>13.77</v>
       </c>
     </row>
-    <row r="130" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>96</v>
       </c>
@@ -43022,12 +43022,12 @@
         <v>3.63</v>
       </c>
     </row>
-    <row r="132" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:132" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="133" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>97</v>
       </c>
@@ -43425,7 +43425,7 @@
         <v>11.62</v>
       </c>
     </row>
-    <row r="134" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>98</v>
       </c>
@@ -43823,7 +43823,7 @@
         <v>2.73</v>
       </c>
     </row>
-    <row r="135" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>99</v>
       </c>
@@ -44221,7 +44221,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="136" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>100</v>
       </c>
@@ -44619,7 +44619,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="137" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>101</v>
       </c>
@@ -45017,7 +45017,7 @@
         <v>4.99</v>
       </c>
     </row>
-    <row r="138" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>102</v>
       </c>
@@ -45415,7 +45415,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="139" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>103</v>
       </c>
@@ -45813,7 +45813,7 @@
         <v>6.99</v>
       </c>
     </row>
-    <row r="140" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>104</v>
       </c>
@@ -46211,7 +46211,7 @@
         <v>6.15</v>
       </c>
     </row>
-    <row r="141" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>105</v>
       </c>
@@ -46609,12 +46609,12 @@
         <v>9.16</v>
       </c>
     </row>
-    <row r="143" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:132" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="144" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>106</v>
       </c>
@@ -47012,7 +47012,7 @@
         <v>7.45</v>
       </c>
     </row>
-    <row r="145" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>107</v>
       </c>
@@ -47410,7 +47410,7 @@
         <v>4.88</v>
       </c>
     </row>
-    <row r="146" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>108</v>
       </c>
@@ -47808,7 +47808,7 @@
         <v>4.1500000000000004</v>
       </c>
     </row>
-    <row r="147" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>109</v>
       </c>
@@ -48206,7 +48206,7 @@
         <v>6.89</v>
       </c>
     </row>
-    <row r="148" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>110</v>
       </c>
@@ -48604,12 +48604,12 @@
         <v>2.09</v>
       </c>
     </row>
-    <row r="150" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:132" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="151" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>111</v>
       </c>
@@ -49007,7 +49007,7 @@
         <v>2.39</v>
       </c>
     </row>
-    <row r="152" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>112</v>
       </c>
@@ -49405,7 +49405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>113</v>
       </c>
@@ -49803,7 +49803,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="155" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>114</v>
       </c>
@@ -50201,7 +50201,7 @@
         <v>5.98</v>
       </c>
     </row>
-    <row r="156" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>115</v>
       </c>
@@ -50599,7 +50599,7 @@
         <v>5.0599999999999996</v>
       </c>
     </row>
-    <row r="157" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>116</v>
       </c>
@@ -50997,7 +50997,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="158" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>117</v>
       </c>
@@ -51395,7 +51395,7 @@
         <v>7.06</v>
       </c>
     </row>
-    <row r="159" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>118</v>
       </c>
@@ -51793,7 +51793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>119</v>
       </c>
@@ -52191,7 +52191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>120</v>
       </c>
@@ -52589,7 +52589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>121</v>
       </c>
@@ -52987,7 +52987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>122</v>
       </c>
@@ -53385,7 +53385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>123</v>
       </c>
@@ -53783,7 +53783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>124</v>
       </c>
@@ -54181,7 +54181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>125</v>
       </c>
@@ -54579,7 +54579,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="171" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>126</v>
       </c>
@@ -54977,7 +54977,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="172" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>127</v>
       </c>
@@ -55375,7 +55375,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="173" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>130</v>
       </c>
@@ -55773,7 +55773,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="174" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>134</v>
       </c>
@@ -56171,7 +56171,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="175" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>135</v>
       </c>
@@ -56569,7 +56569,7 @@
         <v>2.44</v>
       </c>
     </row>
-    <row r="177" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>136</v>
       </c>
@@ -56967,7 +56967,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="179" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>137</v>
       </c>
@@ -57365,7 +57365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>138</v>
       </c>
@@ -57763,7 +57763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>139</v>
       </c>
@@ -58161,7 +58161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>140</v>
       </c>
@@ -58559,7 +58559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>141</v>
       </c>
@@ -58957,7 +58957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>142</v>
       </c>
@@ -59355,12 +59355,12 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="186" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:132" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="187" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>143</v>
       </c>
@@ -59758,7 +59758,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="188" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>144</v>
       </c>
@@ -60156,7 +60156,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="189" spans="1:132" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:132" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>145</v>
       </c>
@@ -60554,74 +60554,74 @@
         <v>1.41</v>
       </c>
     </row>
-    <row r="190" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:132" x14ac:dyDescent="0.25">
       <c r="B190" s="29" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="191" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:132" x14ac:dyDescent="0.25">
       <c r="B191" s="30" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="192" spans="1:132" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:132" x14ac:dyDescent="0.25">
       <c r="B192" s="30" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B193" s="3"/>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B196" s="3" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B197" s="3" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B199" s="31" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B200" s="3"/>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B201" s="3" t="s">
         <v>309</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="M10:Q10"/>
-    <mergeCell ref="R10:V10"/>
-    <mergeCell ref="B1:EB1"/>
-    <mergeCell ref="B2:EB2"/>
-    <mergeCell ref="B3:EB3"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="DI10:DM10"/>
+    <mergeCell ref="DN10:DR10"/>
+    <mergeCell ref="DS10:DW10"/>
+    <mergeCell ref="DX10:EB10"/>
+    <mergeCell ref="CE10:CI10"/>
+    <mergeCell ref="CJ10:CN10"/>
+    <mergeCell ref="CO10:CS10"/>
+    <mergeCell ref="CT10:CX10"/>
+    <mergeCell ref="CY10:DC10"/>
+    <mergeCell ref="DD10:DH10"/>
     <mergeCell ref="BZ10:CD10"/>
     <mergeCell ref="W10:AA10"/>
     <mergeCell ref="AB10:AF10"/>
@@ -60634,16 +60634,16 @@
     <mergeCell ref="BK10:BO10"/>
     <mergeCell ref="BP10:BT10"/>
     <mergeCell ref="BU10:BY10"/>
-    <mergeCell ref="DI10:DM10"/>
-    <mergeCell ref="DN10:DR10"/>
-    <mergeCell ref="DS10:DW10"/>
-    <mergeCell ref="DX10:EB10"/>
-    <mergeCell ref="CE10:CI10"/>
-    <mergeCell ref="CJ10:CN10"/>
-    <mergeCell ref="CO10:CS10"/>
-    <mergeCell ref="CT10:CX10"/>
-    <mergeCell ref="CY10:DC10"/>
-    <mergeCell ref="DD10:DH10"/>
+    <mergeCell ref="B1:EB1"/>
+    <mergeCell ref="B2:EB2"/>
+    <mergeCell ref="B3:EB3"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H10:L10"/>
+    <mergeCell ref="M10:Q10"/>
+    <mergeCell ref="R10:V10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B9:C9" r:id="rId1" display="http://www2.census.gov/govs/state/11_methodology.pdf" xr:uid="{B00DD017-2633-4785-AE59-98CF64D930E7}"/>

</xml_diff>